<commit_message>
Cập nhật file phân tích theo BAchecklist, Bổ sung file phân tích Cập nhật mặt hàng.
</commit_message>
<xml_diff>
--- a/2018/Thao Phuong/02 QL VatTu-MatHang/SOF.QP.04.M05_CF0050_Danh muc mat hang.xlsx
+++ b/2018/Thao Phuong/02 QL VatTu-MatHang/SOF.QP.04.M05_CF0050_Danh muc mat hang.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SVN\THUCTAP\Thao Phuong\02 QL VatTu-MatHang\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Phuong\Analyze\Phương\Done\SVN-GitHub\Thao Phuong\02 QL VatTu-MatHang\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8640" tabRatio="653" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8640" tabRatio="653" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="2" r:id="rId1"/>
@@ -680,7 +680,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11">
     <font>
       <sz val="11"/>
@@ -1073,6 +1073,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1106,15 +1127,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1123,18 +1135,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1315,7 +1315,7 @@
         <xdr:cNvPr id="2" name="Picture 659" descr="Logo 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1367,7 +1367,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1433,7 +1433,7 @@
         <xdr:cNvPr id="2" name="Picture 659" descr="Logo 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1485,7 +1485,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1533,7 +1533,7 @@
         <xdr:cNvPr id="2" name="Picture 659" descr="Logo 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1585,7 +1585,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1651,7 +1651,7 @@
         <xdr:cNvPr id="2" name="Picture 659" descr="Logo 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1703,7 +1703,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1769,7 +1769,7 @@
         <xdr:cNvPr id="2" name="Picture 659" descr="Logo 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1821,7 +1821,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1887,7 +1887,7 @@
         <xdr:cNvPr id="2" name="Picture 659" descr="Logo 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1939,7 +1939,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2061,23 +2061,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2113,23 +2096,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2311,7 +2277,7 @@
   </sheetPr>
   <dimension ref="A1:W48"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A25" zoomScale="85" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="I13" sqref="I13:K13"/>
     </sheetView>
   </sheetViews>
@@ -2339,16 +2305,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="46" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
       <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
@@ -2357,28 +2323,28 @@
       </c>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
       <c r="J2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
       <c r="J3" s="2" t="s">
         <v>27</v>
       </c>
@@ -2465,94 +2431,94 @@
       <c r="H11" s="44"/>
     </row>
     <row r="12" spans="1:23">
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="D12" s="52" t="s">
+      <c r="D12" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="52" t="s">
+      <c r="E12" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="52" t="s">
+      <c r="F12" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="55" t="s">
+      <c r="G12" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="55"/>
-      <c r="I12" s="56" t="s">
+      <c r="H12" s="62"/>
+      <c r="I12" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J12" s="57"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="56" t="s">
+      <c r="J12" s="47"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="M12" s="57"/>
-      <c r="N12" s="58"/>
-      <c r="O12" s="56" t="s">
+      <c r="M12" s="47"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="P12" s="57"/>
-      <c r="Q12" s="58"/>
-      <c r="R12" s="56" t="s">
+      <c r="P12" s="47"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="S12" s="57"/>
-      <c r="T12" s="58"/>
-      <c r="U12" s="56" t="s">
+      <c r="S12" s="47"/>
+      <c r="T12" s="48"/>
+      <c r="U12" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="V12" s="57"/>
-      <c r="W12" s="58"/>
+      <c r="V12" s="47"/>
+      <c r="W12" s="48"/>
     </row>
     <row r="13" spans="1:23">
-      <c r="B13" s="53"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="63" t="s">
+      <c r="B13" s="60"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="H13" s="64"/>
-      <c r="I13" s="63" t="s">
+      <c r="H13" s="50"/>
+      <c r="I13" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="J13" s="65"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="63" t="s">
+      <c r="J13" s="51"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="M13" s="65"/>
-      <c r="N13" s="64"/>
-      <c r="O13" s="63" t="s">
+      <c r="M13" s="51"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="P13" s="65"/>
-      <c r="Q13" s="64"/>
-      <c r="R13" s="63" t="s">
+      <c r="P13" s="51"/>
+      <c r="Q13" s="50"/>
+      <c r="R13" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="S13" s="65"/>
-      <c r="T13" s="64"/>
-      <c r="U13" s="63" t="s">
+      <c r="S13" s="51"/>
+      <c r="T13" s="50"/>
+      <c r="U13" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="V13" s="65"/>
-      <c r="W13" s="64"/>
+      <c r="V13" s="51"/>
+      <c r="W13" s="50"/>
     </row>
     <row r="14" spans="1:23" ht="28.5">
       <c r="A14" s="6"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
       <c r="G14" s="7" t="s">
         <v>17</v>
       </c>
@@ -2646,7 +2612,7 @@
       <c r="C16" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="62" t="s">
+      <c r="D16" s="45" t="s">
         <v>5</v>
       </c>
       <c r="E16" s="19" t="s">
@@ -2678,7 +2644,7 @@
       <c r="C17" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="62"/>
+      <c r="D17" s="45"/>
       <c r="E17" s="18"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
@@ -2706,7 +2672,7 @@
       <c r="C18" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="62"/>
+      <c r="D18" s="45"/>
       <c r="E18" s="18"/>
       <c r="F18" s="13"/>
       <c r="G18" s="11"/>
@@ -2732,7 +2698,7 @@
       <c r="C19" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="62"/>
+      <c r="D19" s="45"/>
       <c r="E19" s="18" t="s">
         <v>100</v>
       </c>
@@ -2764,7 +2730,7 @@
       <c r="C20" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="62"/>
+      <c r="D20" s="45"/>
       <c r="E20" s="25"/>
       <c r="F20" s="13"/>
       <c r="G20" s="11"/>
@@ -2792,7 +2758,7 @@
       <c r="C21" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="62"/>
+      <c r="D21" s="45"/>
       <c r="E21" s="18" t="s">
         <v>40</v>
       </c>
@@ -2824,7 +2790,7 @@
       <c r="C22" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="62"/>
+      <c r="D22" s="45"/>
       <c r="E22" s="18" t="s">
         <v>20</v>
       </c>
@@ -2856,7 +2822,7 @@
       <c r="C23" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D23" s="62"/>
+      <c r="D23" s="45"/>
       <c r="E23" s="18" t="s">
         <v>7</v>
       </c>
@@ -2888,7 +2854,7 @@
       <c r="C24" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="62"/>
+      <c r="D24" s="45"/>
       <c r="E24" s="18" t="s">
         <v>24</v>
       </c>
@@ -2920,7 +2886,7 @@
       <c r="C25" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D25" s="62"/>
+      <c r="D25" s="45"/>
       <c r="E25" s="18" t="s">
         <v>64</v>
       </c>
@@ -2952,7 +2918,7 @@
       <c r="C26" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D26" s="62"/>
+      <c r="D26" s="45"/>
       <c r="E26" s="3" t="s">
         <v>65</v>
       </c>
@@ -3653,6 +3619,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="E1:I3"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="C12:C14"/>
     <mergeCell ref="D16:D26"/>
     <mergeCell ref="L12:N12"/>
     <mergeCell ref="O12:Q12"/>
@@ -3664,15 +3639,6 @@
     <mergeCell ref="O13:Q13"/>
     <mergeCell ref="R13:T13"/>
     <mergeCell ref="U13:W13"/>
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="E1:I3"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="C12:C14"/>
   </mergeCells>
   <conditionalFormatting sqref="G15:G46 I15:J46 L15:M46 O15:P46 R15:S46 U15:V46">
     <cfRule type="expression" dxfId="21" priority="4">
@@ -3744,16 +3710,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="46" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
       <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
@@ -3762,28 +3728,28 @@
       </c>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
       <c r="J2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15.75">
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
       <c r="J3" s="2" t="s">
         <v>27</v>
       </c>
@@ -3852,94 +3818,94 @@
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:23">
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="59" t="s">
+      <c r="C10" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="52" t="s">
+      <c r="D10" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="52" t="s">
+      <c r="E10" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="52" t="s">
+      <c r="F10" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="55" t="s">
+      <c r="G10" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="55"/>
-      <c r="I10" s="56" t="s">
+      <c r="H10" s="62"/>
+      <c r="I10" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="57"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="56" t="s">
+      <c r="J10" s="47"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="M10" s="57"/>
-      <c r="N10" s="58"/>
-      <c r="O10" s="56" t="s">
+      <c r="M10" s="47"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="P10" s="57"/>
-      <c r="Q10" s="58"/>
-      <c r="R10" s="56" t="s">
+      <c r="P10" s="47"/>
+      <c r="Q10" s="48"/>
+      <c r="R10" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="S10" s="57"/>
-      <c r="T10" s="58"/>
-      <c r="U10" s="56" t="s">
+      <c r="S10" s="47"/>
+      <c r="T10" s="48"/>
+      <c r="U10" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="V10" s="57"/>
-      <c r="W10" s="58"/>
+      <c r="V10" s="47"/>
+      <c r="W10" s="48"/>
     </row>
     <row r="11" spans="1:23">
-      <c r="B11" s="53"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="63" t="s">
+      <c r="B11" s="60"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="64"/>
-      <c r="I11" s="63" t="s">
+      <c r="H11" s="50"/>
+      <c r="I11" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="J11" s="65"/>
-      <c r="K11" s="64"/>
-      <c r="L11" s="63" t="s">
+      <c r="J11" s="51"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="M11" s="65"/>
-      <c r="N11" s="64"/>
-      <c r="O11" s="63" t="s">
+      <c r="M11" s="51"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="P11" s="65"/>
-      <c r="Q11" s="64"/>
-      <c r="R11" s="63" t="s">
+      <c r="P11" s="51"/>
+      <c r="Q11" s="50"/>
+      <c r="R11" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="S11" s="65"/>
-      <c r="T11" s="64"/>
-      <c r="U11" s="63" t="s">
+      <c r="S11" s="51"/>
+      <c r="T11" s="50"/>
+      <c r="U11" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="V11" s="65"/>
-      <c r="W11" s="64"/>
+      <c r="V11" s="51"/>
+      <c r="W11" s="50"/>
     </row>
     <row r="12" spans="1:23" ht="28.5">
       <c r="A12" s="6"/>
-      <c r="B12" s="54"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
       <c r="G12" s="7" t="s">
         <v>17</v>
       </c>
@@ -4917,6 +4883,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="U10:W10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="R11:T11"/>
+    <mergeCell ref="U11:W11"/>
     <mergeCell ref="D13:D15"/>
     <mergeCell ref="B1:D3"/>
     <mergeCell ref="E1:I3"/>
@@ -4927,16 +4903,6 @@
     <mergeCell ref="F10:F12"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="I10:K10"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="U10:W10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="O11:Q11"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="U11:W11"/>
   </mergeCells>
   <conditionalFormatting sqref="G13:G43 I13:J43 L13:M43 O13:P43 R13:S43 U13:V43">
     <cfRule type="expression" dxfId="18" priority="4">
@@ -4978,10 +4944,10 @@
   <dimension ref="A1:V49"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="14" topLeftCell="F21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="14" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="G33" sqref="G33"/>
+      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5008,16 +4974,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="46" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
       <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
@@ -5026,28 +4992,28 @@
       </c>
     </row>
     <row r="2" spans="1:22" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
       <c r="J2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:22" s="1" customFormat="1" ht="15.75">
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
       <c r="J3" s="2" t="s">
         <v>27</v>
       </c>
@@ -5134,88 +5100,88 @@
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:22">
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="D12" s="52" t="s">
+      <c r="D12" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="52" t="s">
+      <c r="E12" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="52" t="s">
+      <c r="F12" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="55" t="s">
+      <c r="G12" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="55"/>
-      <c r="I12" s="56" t="s">
+      <c r="H12" s="62"/>
+      <c r="I12" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J12" s="57"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="56" t="s">
+      <c r="J12" s="47"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="O12" s="57"/>
-      <c r="P12" s="58"/>
-      <c r="Q12" s="56" t="s">
+      <c r="O12" s="47"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="R12" s="57"/>
-      <c r="S12" s="58"/>
-      <c r="T12" s="56" t="s">
+      <c r="R12" s="47"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="U12" s="57"/>
-      <c r="V12" s="58"/>
+      <c r="U12" s="47"/>
+      <c r="V12" s="48"/>
     </row>
     <row r="13" spans="1:22">
-      <c r="B13" s="53"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="63" t="s">
+      <c r="B13" s="60"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="64"/>
-      <c r="I13" s="63" t="s">
+      <c r="H13" s="50"/>
+      <c r="I13" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="J13" s="65"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="65"/>
-      <c r="M13" s="64"/>
-      <c r="N13" s="63" t="s">
+      <c r="J13" s="51"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="O13" s="65"/>
-      <c r="P13" s="64"/>
-      <c r="Q13" s="63" t="s">
+      <c r="O13" s="51"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="R13" s="65"/>
-      <c r="S13" s="64"/>
-      <c r="T13" s="63" t="s">
+      <c r="R13" s="51"/>
+      <c r="S13" s="50"/>
+      <c r="T13" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="U13" s="65"/>
-      <c r="V13" s="64"/>
+      <c r="U13" s="51"/>
+      <c r="V13" s="50"/>
     </row>
     <row r="14" spans="1:22" ht="28.5">
       <c r="A14" s="6"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
       <c r="G14" s="7" t="s">
         <v>17</v>
       </c>
@@ -6246,14 +6212,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D15:D20"/>
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="E1:I3"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="C12:C14"/>
     <mergeCell ref="T12:V12"/>
     <mergeCell ref="T13:V13"/>
     <mergeCell ref="N12:P12"/>
@@ -6266,6 +6224,14 @@
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="I13:K13"/>
     <mergeCell ref="L13:M13"/>
+    <mergeCell ref="D15:D20"/>
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="E1:I3"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="C12:C14"/>
   </mergeCells>
   <conditionalFormatting sqref="G15:G45 I15:J45 N15:O45 Q15:R45 T15:U45 L15:L48">
     <cfRule type="expression" dxfId="14" priority="15">
@@ -6306,8 +6272,8 @@
   </sheetPr>
   <dimension ref="A1:W50"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScale="85" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13:K13"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A19" zoomScale="85" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6334,16 +6300,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="46" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
       <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
@@ -6352,28 +6318,28 @@
       </c>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
       <c r="J2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
       <c r="J3" s="2" t="s">
         <v>27</v>
       </c>
@@ -6460,94 +6426,94 @@
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:23">
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="D12" s="52" t="s">
+      <c r="D12" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="52" t="s">
+      <c r="E12" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="52" t="s">
+      <c r="F12" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="55" t="s">
+      <c r="G12" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="55"/>
-      <c r="I12" s="56" t="s">
+      <c r="H12" s="62"/>
+      <c r="I12" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J12" s="57"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="56" t="s">
+      <c r="J12" s="47"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="M12" s="57"/>
-      <c r="N12" s="58"/>
-      <c r="O12" s="56" t="s">
+      <c r="M12" s="47"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="P12" s="57"/>
-      <c r="Q12" s="58"/>
-      <c r="R12" s="56" t="s">
+      <c r="P12" s="47"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="S12" s="57"/>
-      <c r="T12" s="58"/>
-      <c r="U12" s="56" t="s">
+      <c r="S12" s="47"/>
+      <c r="T12" s="48"/>
+      <c r="U12" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="V12" s="57"/>
-      <c r="W12" s="58"/>
+      <c r="V12" s="47"/>
+      <c r="W12" s="48"/>
     </row>
     <row r="13" spans="1:23">
-      <c r="B13" s="53"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="63" t="s">
+      <c r="B13" s="60"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="H13" s="64"/>
-      <c r="I13" s="63" t="s">
+      <c r="H13" s="50"/>
+      <c r="I13" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="J13" s="65"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="63" t="s">
+      <c r="J13" s="51"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="M13" s="65"/>
-      <c r="N13" s="64"/>
-      <c r="O13" s="63" t="s">
+      <c r="M13" s="51"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="P13" s="65"/>
-      <c r="Q13" s="64"/>
-      <c r="R13" s="63" t="s">
+      <c r="P13" s="51"/>
+      <c r="Q13" s="50"/>
+      <c r="R13" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="S13" s="65"/>
-      <c r="T13" s="64"/>
-      <c r="U13" s="63" t="s">
+      <c r="S13" s="51"/>
+      <c r="T13" s="50"/>
+      <c r="U13" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="V13" s="65"/>
-      <c r="W13" s="64"/>
+      <c r="V13" s="51"/>
+      <c r="W13" s="50"/>
     </row>
     <row r="14" spans="1:23" ht="28.5">
       <c r="A14" s="6"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
       <c r="G14" s="7" t="s">
         <v>17</v>
       </c>
@@ -7700,6 +7666,21 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="D30:D36"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E1:I3"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="C12:C14"/>
     <mergeCell ref="U12:W12"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="I13:K13"/>
@@ -7710,21 +7691,6 @@
     <mergeCell ref="L12:N12"/>
     <mergeCell ref="O12:Q12"/>
     <mergeCell ref="R12:T12"/>
-    <mergeCell ref="E1:I3"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="D30:D36"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D24:D25"/>
   </mergeCells>
   <conditionalFormatting sqref="G15:G48 I15:J48 L15:M48 O15:P48 R15:S48 U15:V48">
     <cfRule type="expression" dxfId="10" priority="4">
@@ -7794,16 +7760,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="46" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
       <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
@@ -7812,28 +7778,28 @@
       </c>
     </row>
     <row r="2" spans="1:22" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
       <c r="J2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:22" s="1" customFormat="1" ht="15.75">
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
       <c r="J3" s="2" t="s">
         <v>27</v>
       </c>
@@ -7920,88 +7886,88 @@
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:22">
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="D12" s="52" t="s">
+      <c r="D12" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="52" t="s">
+      <c r="E12" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="52" t="s">
+      <c r="F12" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="55" t="s">
+      <c r="G12" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="55"/>
-      <c r="I12" s="56" t="s">
+      <c r="H12" s="62"/>
+      <c r="I12" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J12" s="57"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="56" t="s">
+      <c r="J12" s="47"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="O12" s="57"/>
-      <c r="P12" s="58"/>
-      <c r="Q12" s="56" t="s">
+      <c r="O12" s="47"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="R12" s="57"/>
-      <c r="S12" s="58"/>
-      <c r="T12" s="56" t="s">
+      <c r="R12" s="47"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="U12" s="57"/>
-      <c r="V12" s="58"/>
+      <c r="U12" s="47"/>
+      <c r="V12" s="48"/>
     </row>
     <row r="13" spans="1:22">
-      <c r="B13" s="53"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="63" t="s">
+      <c r="B13" s="60"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="64"/>
-      <c r="I13" s="63" t="s">
+      <c r="H13" s="50"/>
+      <c r="I13" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="J13" s="65"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="65"/>
-      <c r="M13" s="64"/>
-      <c r="N13" s="63" t="s">
+      <c r="J13" s="51"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="O13" s="65"/>
-      <c r="P13" s="64"/>
-      <c r="Q13" s="63" t="s">
+      <c r="O13" s="51"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="R13" s="65"/>
-      <c r="S13" s="64"/>
-      <c r="T13" s="63" t="s">
+      <c r="R13" s="51"/>
+      <c r="S13" s="50"/>
+      <c r="T13" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="U13" s="65"/>
-      <c r="V13" s="64"/>
+      <c r="U13" s="51"/>
+      <c r="V13" s="50"/>
     </row>
     <row r="14" spans="1:22" ht="28.5">
       <c r="A14" s="6"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
       <c r="G14" s="7" t="s">
         <v>17</v>
       </c>
@@ -8927,15 +8893,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="E1:I3"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:K12"/>
     <mergeCell ref="L12:M12"/>
     <mergeCell ref="N12:P12"/>
     <mergeCell ref="Q12:S12"/>
@@ -8946,6 +8903,15 @@
     <mergeCell ref="N13:P13"/>
     <mergeCell ref="Q13:S13"/>
     <mergeCell ref="T13:V13"/>
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="E1:I3"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:K12"/>
   </mergeCells>
   <conditionalFormatting sqref="G15:G45 I15:J45 N15:O45 Q15:R45 T15:U45 L15:L48">
     <cfRule type="expression" dxfId="7" priority="4">
@@ -8986,7 +8952,7 @@
   </sheetPr>
   <dimension ref="A1:V49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
@@ -9013,15 +8979,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="46" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
       <c r="I1" s="2" t="s">
         <v>25</v>
       </c>
@@ -9030,26 +8996,26 @@
       </c>
     </row>
     <row r="2" spans="1:22" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
       <c r="I2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:22" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
       <c r="I3" s="2" t="s">
         <v>27</v>
       </c>
@@ -9131,89 +9097,89 @@
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:22">
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="52" t="s">
+      <c r="C12" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="52" t="s">
+      <c r="D12" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="52" t="s">
+      <c r="E12" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="55" t="s">
+      <c r="F12" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="55"/>
-      <c r="H12" s="56" t="s">
+      <c r="G12" s="62"/>
+      <c r="H12" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="57"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="56" t="s">
+      <c r="I12" s="47"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="L12" s="57"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="56" t="s">
+      <c r="L12" s="47"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="O12" s="57"/>
-      <c r="P12" s="58"/>
-      <c r="Q12" s="56" t="s">
+      <c r="O12" s="47"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="R12" s="57"/>
-      <c r="S12" s="58"/>
-      <c r="T12" s="56" t="s">
+      <c r="R12" s="47"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="U12" s="57"/>
-      <c r="V12" s="58"/>
+      <c r="U12" s="47"/>
+      <c r="V12" s="48"/>
     </row>
     <row r="13" spans="1:22">
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="63" t="s">
+      <c r="B13" s="60"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="64"/>
-      <c r="H13" s="63" t="s">
+      <c r="G13" s="50"/>
+      <c r="H13" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="I13" s="65"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="63" t="s">
+      <c r="I13" s="51"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="L13" s="65"/>
-      <c r="M13" s="64"/>
-      <c r="N13" s="63" t="s">
+      <c r="L13" s="51"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="O13" s="65"/>
-      <c r="P13" s="64"/>
-      <c r="Q13" s="63" t="s">
+      <c r="O13" s="51"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="R13" s="65"/>
-      <c r="S13" s="64"/>
-      <c r="T13" s="63" t="s">
+      <c r="R13" s="51"/>
+      <c r="S13" s="50"/>
+      <c r="T13" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="U13" s="65"/>
-      <c r="V13" s="64"/>
+      <c r="U13" s="51"/>
+      <c r="V13" s="50"/>
     </row>
     <row r="14" spans="1:22" ht="28.5">
       <c r="A14" s="6"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
       <c r="F14" s="7" t="s">
         <v>17</v>
       </c>
@@ -10156,6 +10122,15 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C15:C21"/>
+    <mergeCell ref="B1:C3"/>
+    <mergeCell ref="D1:H3"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:J12"/>
     <mergeCell ref="K12:M12"/>
     <mergeCell ref="N12:P12"/>
     <mergeCell ref="Q12:S12"/>
@@ -10166,15 +10141,6 @@
     <mergeCell ref="N13:P13"/>
     <mergeCell ref="Q13:S13"/>
     <mergeCell ref="T13:V13"/>
-    <mergeCell ref="C15:C21"/>
-    <mergeCell ref="B1:C3"/>
-    <mergeCell ref="D1:H3"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:J12"/>
   </mergeCells>
   <conditionalFormatting sqref="F15:F45 H15:I45 K15:L45 N15:O45 Q15:R45 T15:U45">
     <cfRule type="expression" dxfId="3" priority="4">

</xml_diff>